<commit_message>
Initial PMA data commit
</commit_message>
<xml_diff>
--- a/data/pma/source data/O'Keeffe Linked.Art PMA 7-31-19.xlsx
+++ b/data/pma/source data/O'Keeffe Linked.Art PMA 7-31-19.xlsx
@@ -1958,7 +1958,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1969,8 +1969,8 @@
   <dimension ref="A1:S95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I3" sqref="I3"/>
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>